<commit_message>
Alt skal nå beregnes riktig
</commit_message>
<xml_diff>
--- a/Prissatser_Nettleie_Alle.xlsx
+++ b/Prissatser_Nettleie_Alle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asmund.fossum\Documents\Strompriser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91630AD-D3E0-442A-A0ED-047C05933D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B0D4B7-200C-4AF0-B150-FE028FB68D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-120" windowWidth="30936" windowHeight="16776" xr2:uid="{6FA07EE8-6DA0-4D58-82CD-6C71EA6AED72}"/>
+    <workbookView xWindow="-30828" yWindow="-120" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{6FA07EE8-6DA0-4D58-82CD-6C71EA6AED72}"/>
   </bookViews>
   <sheets>
     <sheet name="Privatkunde" sheetId="3" r:id="rId1"/>
@@ -386,12 +386,6 @@
     <t>Nettleiepriser mindre bedriftskunder</t>
   </si>
   <si>
-    <t>Enovaavgift/
-energifondsavgift 
-Skal IKKE inkluderes i
-kapasitetsledd</t>
-  </si>
-  <si>
     <t>Nettsiden inkluderer 800 kr/år i kapledd</t>
   </si>
   <si>
@@ -399,6 +393,10 @@
   </si>
   <si>
     <t>Nettselskap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enovaavgift/
+energifondsavgift </t>
   </si>
 </sst>
 </file>
@@ -406,7 +404,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -588,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -609,22 +607,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
@@ -641,6 +634,351 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TekstSylinder 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1618C77-8BF8-B62C-FC14-DAF4ED55E76F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16238220" y="6499860"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="nb-NO" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>15241</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>45721</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2964180" cy="1767840"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TekstSylinder 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A1D4F83-7443-0A8D-63C2-EC5B664815AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16047721" y="6263641"/>
+          <a:ext cx="2964180" cy="1767840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Dersom nettselskapet oppgir Energiledd inkl. avgifter og </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>mva. for</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> (jan-mar) og (apr-des) hver for seg:</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="nb-NO" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:br>
+            <a:rPr lang="nb-NO" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Fyll inn kun verdiene for (apr-des) og sett Forbruksavgift/elavgift (jan-mar) lik den for apr-des, altså 20.55 i stedet for 11.89.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="nb-NO" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:br>
+            <a:rPr lang="nb-NO" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Da beregnes alt riktig</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="nb-NO" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1376082" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TekstSylinder 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11A87483-0FFA-C55F-D910-3D21087DB752}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28956000" y="6248400"/>
+          <a:ext cx="1376082" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" kern="1200"/>
+            <a:t>Skal IKKE inkluderes i</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1100" kern="1200"/>
+            <a:t>energiledd</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -962,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B62DA51-71C0-43EF-B7F9-1F75FC2FFE75}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -986,7 +1324,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>39</v>
@@ -1033,7 +1371,7 @@
       <c r="P1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="18" t="s">
         <v>54</v>
       </c>
       <c r="R1" s="6" t="s">
@@ -1110,7 +1448,7 @@
       <c r="P2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="22" t="s">
+      <c r="Q2" s="19" t="s">
         <v>20</v>
       </c>
       <c r="R2" s="9" t="s">
@@ -1154,40 +1492,40 @@
       <c r="E3" s="1">
         <v>601</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="1">
         <v>794</v>
       </c>
       <c r="G3" s="1">
         <v>989</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="1">
         <v>1699</v>
       </c>
       <c r="I3" s="1">
         <v>2667</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="1">
         <v>3635</v>
       </c>
       <c r="K3" s="1">
         <v>5250</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="1">
         <v>7185</v>
       </c>
       <c r="M3" s="1">
         <v>10411</v>
       </c>
-      <c r="N3" s="16">
+      <c r="N3" s="1">
         <v>14288</v>
       </c>
       <c r="O3" s="1">
         <v>18158</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3" s="1">
         <v>22032</v>
       </c>
-      <c r="Q3" s="23">
+      <c r="Q3" s="20">
         <v>50.18</v>
       </c>
       <c r="R3" s="1">
@@ -1199,7 +1537,7 @@
       <c r="T3" s="12">
         <v>20.55</v>
       </c>
-      <c r="U3" s="25">
+      <c r="U3" s="13">
         <v>20.55</v>
       </c>
       <c r="V3" s="12">
@@ -1208,10 +1546,10 @@
       <c r="W3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="X3" s="18">
+      <c r="X3" s="16">
         <v>45601</v>
       </c>
-      <c r="Y3" s="19" t="s">
+      <c r="Y3" s="17" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1231,40 +1569,40 @@
       <c r="E4" s="1">
         <v>760</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="1">
         <v>990</v>
       </c>
       <c r="G4" s="1">
         <v>1240</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="1">
         <v>1920</v>
       </c>
       <c r="I4" s="1">
         <v>3040</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="1">
         <v>4050</v>
       </c>
       <c r="K4" s="1">
         <v>6580</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="1">
         <v>6580</v>
       </c>
       <c r="M4" s="1">
         <v>6580</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N4" s="1">
         <v>6580</v>
       </c>
       <c r="O4" s="1">
         <v>6580</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="1">
         <v>6580</v>
       </c>
-      <c r="Q4" s="23">
+      <c r="Q4" s="20">
         <v>53</v>
       </c>
       <c r="R4" s="1">
@@ -1276,7 +1614,7 @@
       <c r="T4" s="12">
         <v>11.89</v>
       </c>
-      <c r="U4" s="25">
+      <c r="U4" s="13">
         <v>20.55</v>
       </c>
       <c r="V4" s="12">
@@ -1285,10 +1623,10 @@
       <c r="W4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="X4" s="18">
+      <c r="X4" s="16">
         <v>45601</v>
       </c>
-      <c r="Y4" s="19" t="s">
+      <c r="Y4" s="17" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1308,40 +1646,40 @@
       <c r="E5" s="1">
         <v>620</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="1">
         <v>800</v>
       </c>
       <c r="G5" s="1">
         <v>975</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="1">
         <v>1870</v>
       </c>
       <c r="I5" s="1">
         <v>2760</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="1">
         <v>3650</v>
       </c>
       <c r="K5" s="1">
         <v>7200</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="1">
         <v>7200</v>
       </c>
       <c r="M5" s="1">
         <v>7200</v>
       </c>
-      <c r="N5" s="16">
+      <c r="N5" s="1">
         <v>7200</v>
       </c>
       <c r="O5" s="1">
         <v>7200</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5" s="1">
         <v>7200</v>
       </c>
-      <c r="Q5" s="23">
+      <c r="Q5" s="20">
         <v>59.25</v>
       </c>
       <c r="R5" s="1">
@@ -1351,9 +1689,9 @@
         <v>63</v>
       </c>
       <c r="T5" s="12">
-        <v>11.89</v>
-      </c>
-      <c r="U5" s="25">
+        <v>20.55</v>
+      </c>
+      <c r="U5" s="13">
         <v>20.55</v>
       </c>
       <c r="V5" s="12">
@@ -1362,10 +1700,10 @@
       <c r="W5" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="X5" s="18">
+      <c r="X5" s="16">
         <v>45601</v>
       </c>
-      <c r="Y5" s="19" t="s">
+      <c r="Y5" s="17" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1385,25 +1723,25 @@
       <c r="E6" s="1">
         <v>707.5</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="1">
         <v>916.5</v>
       </c>
       <c r="G6" s="1">
         <v>1123.75</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="1">
         <v>1746.25</v>
       </c>
       <c r="I6" s="1">
         <v>2783.75</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="1">
         <v>3820</v>
       </c>
       <c r="K6" s="1">
         <v>5376.25</v>
       </c>
-      <c r="L6" s="16">
+      <c r="L6" s="1">
         <v>7450</v>
       </c>
       <c r="M6" s="1">
@@ -1418,7 +1756,7 @@
       <c r="P6" s="1">
         <v>10562.5</v>
       </c>
-      <c r="Q6" s="23">
+      <c r="Q6" s="20">
         <v>30.48</v>
       </c>
       <c r="R6" s="1">
@@ -1430,7 +1768,7 @@
       <c r="T6" s="12">
         <v>11.89</v>
       </c>
-      <c r="U6" s="25">
+      <c r="U6" s="13">
         <v>20.55</v>
       </c>
       <c r="V6" s="12">
@@ -1439,10 +1777,10 @@
       <c r="W6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="X6" s="18">
+      <c r="X6" s="16">
         <v>45601</v>
       </c>
-      <c r="Y6" s="19" t="s">
+      <c r="Y6" s="17" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1462,40 +1800,40 @@
       <c r="E7" s="1">
         <v>525</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="1">
         <v>675</v>
       </c>
       <c r="G7" s="1">
         <v>820</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="1">
         <v>1560</v>
       </c>
       <c r="I7" s="1">
         <v>2300</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="1">
         <v>3030</v>
       </c>
       <c r="K7" s="1">
         <v>6050</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="1">
         <v>6050</v>
       </c>
       <c r="M7" s="1">
         <v>6050</v>
       </c>
-      <c r="N7" s="16">
+      <c r="N7" s="1">
         <v>6050</v>
       </c>
       <c r="O7" s="1">
         <v>6050</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="1">
         <v>6050</v>
       </c>
-      <c r="Q7" s="23">
+      <c r="Q7" s="20">
         <v>52.5</v>
       </c>
       <c r="R7" s="1">
@@ -1507,7 +1845,7 @@
       <c r="T7" s="12">
         <v>20.55</v>
       </c>
-      <c r="U7" s="25">
+      <c r="U7" s="13">
         <v>20.55</v>
       </c>
       <c r="V7" s="12">
@@ -1516,10 +1854,10 @@
       <c r="W7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="X7" s="18">
+      <c r="X7" s="16">
         <v>45601</v>
       </c>
-      <c r="Y7" s="19" t="s">
+      <c r="Y7" s="17" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1532,13 +1870,12 @@
       <c r="K8" s="1"/>
       <c r="M8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="23"/>
+      <c r="Q8" s="20"/>
       <c r="R8" s="1"/>
       <c r="T8" s="12">
         <v>11.89</v>
       </c>
-      <c r="U8" s="25">
+      <c r="U8" s="13">
         <v>20.55</v>
       </c>
       <c r="V8" s="12">
@@ -1557,13 +1894,12 @@
       <c r="K9" s="1"/>
       <c r="M9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="23"/>
+      <c r="Q9" s="20"/>
       <c r="R9" s="1"/>
       <c r="T9" s="12">
         <v>11.89</v>
       </c>
-      <c r="U9" s="25">
+      <c r="U9" s="13">
         <v>20.55</v>
       </c>
       <c r="V9" s="12">
@@ -1582,13 +1918,12 @@
       <c r="K10" s="1"/>
       <c r="M10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="23"/>
+      <c r="Q10" s="20"/>
       <c r="R10" s="1"/>
       <c r="T10" s="12">
         <v>11.89</v>
       </c>
-      <c r="U10" s="25">
+      <c r="U10" s="13">
         <v>20.55</v>
       </c>
       <c r="V10" s="12">
@@ -1607,13 +1942,12 @@
       <c r="K11" s="1"/>
       <c r="M11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="23"/>
+      <c r="Q11" s="20"/>
       <c r="R11" s="1"/>
       <c r="T11" s="12">
         <v>11.89</v>
       </c>
-      <c r="U11" s="25">
+      <c r="U11" s="13">
         <v>20.55</v>
       </c>
       <c r="V11" s="12">
@@ -1632,13 +1966,12 @@
       <c r="K12" s="1"/>
       <c r="M12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="23"/>
+      <c r="Q12" s="20"/>
       <c r="R12" s="1"/>
       <c r="T12" s="12">
         <v>11.89</v>
       </c>
-      <c r="U12" s="25">
+      <c r="U12" s="13">
         <v>20.55</v>
       </c>
       <c r="V12" s="12">
@@ -1657,13 +1990,12 @@
       <c r="K13" s="1"/>
       <c r="M13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="23"/>
+      <c r="Q13" s="20"/>
       <c r="R13" s="1"/>
       <c r="T13" s="12">
         <v>11.89</v>
       </c>
-      <c r="U13" s="25">
+      <c r="U13" s="13">
         <v>20.55</v>
       </c>
       <c r="V13" s="12">
@@ -1682,13 +2014,12 @@
       <c r="K14" s="1"/>
       <c r="M14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="23"/>
+      <c r="Q14" s="20"/>
       <c r="R14" s="1"/>
       <c r="T14" s="12">
         <v>11.89</v>
       </c>
-      <c r="U14" s="25">
+      <c r="U14" s="13">
         <v>20.55</v>
       </c>
       <c r="V14" s="12">
@@ -1707,13 +2038,12 @@
       <c r="K15" s="1"/>
       <c r="M15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="23"/>
+      <c r="Q15" s="20"/>
       <c r="R15" s="1"/>
       <c r="T15" s="12">
         <v>11.89</v>
       </c>
-      <c r="U15" s="25">
+      <c r="U15" s="13">
         <v>20.55</v>
       </c>
       <c r="V15" s="12">
@@ -1732,13 +2062,12 @@
       <c r="K16" s="1"/>
       <c r="M16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="23"/>
+      <c r="Q16" s="20"/>
       <c r="R16" s="1"/>
       <c r="T16" s="12">
         <v>11.89</v>
       </c>
-      <c r="U16" s="25">
+      <c r="U16" s="13">
         <v>20.55</v>
       </c>
       <c r="V16" s="12">
@@ -1757,13 +2086,12 @@
       <c r="K17" s="1"/>
       <c r="M17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="23"/>
+      <c r="Q17" s="20"/>
       <c r="R17" s="1"/>
       <c r="T17" s="12">
         <v>11.89</v>
       </c>
-      <c r="U17" s="25">
+      <c r="U17" s="13">
         <v>20.55</v>
       </c>
       <c r="V17" s="12">
@@ -1782,13 +2110,12 @@
       <c r="K18" s="1"/>
       <c r="M18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="23"/>
+      <c r="Q18" s="20"/>
       <c r="R18" s="1"/>
       <c r="T18" s="12">
         <v>11.89</v>
       </c>
-      <c r="U18" s="25">
+      <c r="U18" s="13">
         <v>20.55</v>
       </c>
       <c r="V18" s="12">
@@ -1807,13 +2134,12 @@
       <c r="K19" s="1"/>
       <c r="M19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="23"/>
+      <c r="Q19" s="20"/>
       <c r="R19" s="1"/>
       <c r="T19" s="12">
         <v>11.89</v>
       </c>
-      <c r="U19" s="25">
+      <c r="U19" s="13">
         <v>20.55</v>
       </c>
       <c r="V19" s="12">
@@ -1832,13 +2158,12 @@
       <c r="K20" s="1"/>
       <c r="M20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="23"/>
+      <c r="Q20" s="20"/>
       <c r="R20" s="1"/>
       <c r="T20" s="12">
         <v>11.89</v>
       </c>
-      <c r="U20" s="25">
+      <c r="U20" s="13">
         <v>20.55</v>
       </c>
       <c r="V20" s="12">
@@ -1857,13 +2182,12 @@
       <c r="K21" s="1"/>
       <c r="M21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="23"/>
+      <c r="Q21" s="20"/>
       <c r="R21" s="1"/>
       <c r="T21" s="12">
         <v>11.89</v>
       </c>
-      <c r="U21" s="25">
+      <c r="U21" s="13">
         <v>20.55</v>
       </c>
       <c r="V21" s="12">
@@ -1882,13 +2206,12 @@
       <c r="K22" s="1"/>
       <c r="M22" s="1"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="23"/>
+      <c r="Q22" s="20"/>
       <c r="R22" s="1"/>
       <c r="T22" s="12">
         <v>11.89</v>
       </c>
-      <c r="U22" s="25">
+      <c r="U22" s="13">
         <v>20.55</v>
       </c>
       <c r="V22" s="12">
@@ -1907,13 +2230,12 @@
       <c r="K23" s="1"/>
       <c r="M23" s="1"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="23"/>
+      <c r="Q23" s="20"/>
       <c r="R23" s="1"/>
       <c r="T23" s="12">
         <v>11.89</v>
       </c>
-      <c r="U23" s="25">
+      <c r="U23" s="13">
         <v>20.55</v>
       </c>
       <c r="V23" s="12">
@@ -1932,13 +2254,12 @@
       <c r="K24" s="1"/>
       <c r="M24" s="1"/>
       <c r="O24" s="1"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="23"/>
+      <c r="Q24" s="20"/>
       <c r="R24" s="1"/>
       <c r="T24" s="12">
         <v>11.89</v>
       </c>
-      <c r="U24" s="25">
+      <c r="U24" s="13">
         <v>20.55</v>
       </c>
       <c r="V24" s="12">
@@ -1957,13 +2278,12 @@
       <c r="K25" s="1"/>
       <c r="M25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="23"/>
+      <c r="Q25" s="20"/>
       <c r="R25" s="1"/>
       <c r="T25" s="12">
         <v>11.89</v>
       </c>
-      <c r="U25" s="25">
+      <c r="U25" s="13">
         <v>20.55</v>
       </c>
       <c r="V25" s="12">
@@ -1982,13 +2302,12 @@
       <c r="K26" s="1"/>
       <c r="M26" s="1"/>
       <c r="O26" s="1"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="23"/>
+      <c r="Q26" s="20"/>
       <c r="R26" s="1"/>
       <c r="T26" s="12">
         <v>11.89</v>
       </c>
-      <c r="U26" s="25">
+      <c r="U26" s="13">
         <v>20.55</v>
       </c>
       <c r="V26" s="12">
@@ -2007,13 +2326,12 @@
       <c r="K27" s="1"/>
       <c r="M27" s="1"/>
       <c r="O27" s="1"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="23"/>
+      <c r="Q27" s="20"/>
       <c r="R27" s="1"/>
       <c r="T27" s="12">
         <v>11.89</v>
       </c>
-      <c r="U27" s="25">
+      <c r="U27" s="13">
         <v>20.55</v>
       </c>
       <c r="V27" s="12">
@@ -2032,13 +2350,12 @@
       <c r="K28" s="1"/>
       <c r="M28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="23"/>
+      <c r="Q28" s="20"/>
       <c r="R28" s="1"/>
       <c r="T28" s="12">
         <v>11.89</v>
       </c>
-      <c r="U28" s="25">
+      <c r="U28" s="13">
         <v>20.55</v>
       </c>
       <c r="V28" s="12">
@@ -2057,13 +2374,12 @@
       <c r="K29" s="1"/>
       <c r="M29" s="1"/>
       <c r="O29" s="1"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="23"/>
+      <c r="Q29" s="20"/>
       <c r="R29" s="1"/>
       <c r="T29" s="12">
         <v>11.89</v>
       </c>
-      <c r="U29" s="25">
+      <c r="U29" s="13">
         <v>20.55</v>
       </c>
       <c r="V29" s="12">
@@ -2090,7 +2406,7 @@
       <c r="N30" s="4"/>
       <c r="O30" s="2"/>
       <c r="P30" s="4"/>
-      <c r="Q30" s="23"/>
+      <c r="Q30" s="20"/>
       <c r="R30" s="2"/>
       <c r="S30" s="4"/>
       <c r="T30" s="14">
@@ -2107,7 +2423,7 @@
       <c r="Y30" s="2"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2118,6 +2434,7 @@
     <hyperlink ref="Y7" r:id="rId5" display="https://www.elvia.no/nettleie/alt-om-nettleiepriser/nettleiepriser-for-privatkunder/" xr:uid="{A687149B-F62A-49A2-AB98-24E19224A673}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -2125,8 +2442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0E751E5-E144-4EB0-8D1B-0F591B3C3BE2}">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="W35" sqref="W35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2158,7 +2475,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>69</v>
@@ -2205,7 +2522,7 @@
       <c r="P1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="18" t="s">
         <v>84</v>
       </c>
       <c r="R1" s="6" t="s">
@@ -2224,7 +2541,7 @@
         <v>90</v>
       </c>
       <c r="W1" s="6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="X1" s="6" t="s">
         <v>31</v>
@@ -2285,7 +2602,7 @@
       <c r="P2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="22" t="s">
+      <c r="Q2" s="19" t="s">
         <v>20</v>
       </c>
       <c r="R2" s="9" t="s">
@@ -2332,40 +2649,40 @@
       <c r="E3" s="1">
         <v>480.8</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="1">
         <v>635.20000000000005</v>
       </c>
       <c r="G3" s="1">
         <v>791.2</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="1">
         <v>1359.2</v>
       </c>
       <c r="I3" s="1">
         <v>2133.6</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="1">
         <v>2908</v>
       </c>
       <c r="K3" s="1">
         <v>4200</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="1">
         <v>5748</v>
       </c>
       <c r="M3" s="1">
         <v>8328.7999999999993</v>
       </c>
-      <c r="N3" s="16">
+      <c r="N3" s="1">
         <v>11430.4</v>
       </c>
       <c r="O3" s="1">
         <v>14526.4</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3" s="1">
         <v>17625.599999999999</v>
       </c>
-      <c r="Q3" s="23">
+      <c r="Q3" s="20">
         <v>22.7</v>
       </c>
       <c r="R3" s="1">
@@ -2389,10 +2706,10 @@
       <c r="X3" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="Y3" s="18">
+      <c r="Y3" s="16">
         <v>45601</v>
       </c>
-      <c r="Z3" s="19" t="s">
+      <c r="Z3" s="17" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2412,40 +2729,40 @@
       <c r="E4" s="1">
         <v>608</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="1">
         <v>792</v>
       </c>
       <c r="G4" s="1">
         <v>992</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="1">
         <v>1536</v>
       </c>
       <c r="I4" s="1">
         <v>2432</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="1">
         <v>3240</v>
       </c>
       <c r="K4" s="1">
         <v>5264</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="1">
         <v>5264</v>
       </c>
       <c r="M4" s="1">
         <v>5264</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N4" s="1">
         <v>5264</v>
       </c>
       <c r="O4" s="1">
         <v>5264</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="1">
         <v>5264</v>
       </c>
-      <c r="Q4" s="23">
+      <c r="Q4" s="20">
         <v>24.96</v>
       </c>
       <c r="R4" s="1">
@@ -2467,10 +2784,10 @@
         <v>800</v>
       </c>
       <c r="X4" s="12"/>
-      <c r="Y4" s="18">
+      <c r="Y4" s="16">
         <v>45601</v>
       </c>
-      <c r="Z4" s="19" t="s">
+      <c r="Z4" s="17" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2490,40 +2807,40 @@
       <c r="E5" s="1">
         <v>496</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="1">
         <v>640</v>
       </c>
       <c r="G5" s="1">
         <v>780</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="1">
         <v>1496</v>
       </c>
       <c r="I5" s="1">
         <v>2208</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="1">
         <v>2920</v>
       </c>
       <c r="K5" s="1">
         <v>5760</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="1">
         <v>5760</v>
       </c>
       <c r="M5" s="1">
         <v>5760</v>
       </c>
-      <c r="N5" s="16">
+      <c r="N5" s="1">
         <v>5760</v>
       </c>
       <c r="O5" s="1">
         <v>5760</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5" s="1">
         <v>5760</v>
       </c>
-      <c r="Q5" s="23">
+      <c r="Q5" s="20">
         <v>29.96</v>
       </c>
       <c r="R5" s="1">
@@ -2545,10 +2862,10 @@
         <v>800</v>
       </c>
       <c r="X5" s="12"/>
-      <c r="Y5" s="18">
+      <c r="Y5" s="16">
         <v>45601</v>
       </c>
-      <c r="Z5" s="19" t="s">
+      <c r="Z5" s="17" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2568,25 +2885,25 @@
       <c r="E6" s="1">
         <v>566</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="1">
         <v>733</v>
       </c>
       <c r="G6" s="1">
         <v>899</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="1">
         <v>1397</v>
       </c>
       <c r="I6" s="1">
         <v>2227</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="1">
         <v>3056</v>
       </c>
       <c r="K6" s="1">
         <v>4301</v>
       </c>
-      <c r="L6" s="16">
+      <c r="L6" s="1">
         <v>5960</v>
       </c>
       <c r="M6" s="1">
@@ -2601,7 +2918,7 @@
       <c r="P6" s="1">
         <v>8450</v>
       </c>
-      <c r="Q6" s="23">
+      <c r="Q6" s="20">
         <v>24.38</v>
       </c>
       <c r="R6" s="1">
@@ -2623,10 +2940,10 @@
         <v>800</v>
       </c>
       <c r="X6" s="12"/>
-      <c r="Y6" s="18">
+      <c r="Y6" s="16">
         <v>45601</v>
       </c>
-      <c r="Z6" s="19" t="s">
+      <c r="Z6" s="17" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2634,52 +2951,52 @@
       <c r="A7" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="23">
         <v>112.00333333333332</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="24">
         <v>184.00333333333333</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="23">
         <v>300.00333333333333</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="24">
         <v>420.00333333333333</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="24">
         <v>540.00333333333333</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="24">
         <v>656.00333333333333</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="24">
         <v>1247.6933333333332</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I7" s="24">
         <v>1840.0033333333333</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="24">
         <v>2424.0033333333336</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="24">
         <v>4840.0033333333331</v>
       </c>
-      <c r="L7" s="29">
+      <c r="L7" s="24">
         <v>4840.0033333333331</v>
       </c>
-      <c r="M7" s="28">
+      <c r="M7" s="24">
         <v>4840.0033333333331</v>
       </c>
-      <c r="N7" s="29">
+      <c r="N7" s="24">
         <v>4840.0033333333331</v>
       </c>
-      <c r="O7" s="28">
+      <c r="O7" s="24">
         <v>4840.0033333333331</v>
       </c>
-      <c r="P7" s="29">
+      <c r="P7" s="24">
         <v>4840.0033333333331</v>
       </c>
-      <c r="Q7" s="23">
+      <c r="Q7" s="20">
         <v>24.56</v>
       </c>
       <c r="R7" s="1">
@@ -2701,18 +3018,18 @@
         <v>800</v>
       </c>
       <c r="X7" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y7" s="16">
+        <v>45601</v>
+      </c>
+      <c r="Z7" s="17" t="s">
         <v>94</v>
-      </c>
-      <c r="Y7" s="18">
-        <v>45601</v>
-      </c>
-      <c r="Z7" s="19" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
-      <c r="Q8" s="23"/>
+      <c r="Q8" s="20"/>
       <c r="R8" s="1"/>
       <c r="T8" s="12">
         <v>9.51</v>
@@ -2734,18 +3051,18 @@
       <c r="A9" s="10"/>
       <c r="C9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="16"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="16"/>
+      <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="16"/>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="23"/>
+      <c r="Q9" s="20"/>
       <c r="R9" s="1"/>
       <c r="T9" s="12">
         <v>9.51</v>
@@ -2772,8 +3089,7 @@
       <c r="K10" s="1"/>
       <c r="M10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="23"/>
+      <c r="Q10" s="20"/>
       <c r="R10" s="1"/>
       <c r="T10" s="12">
         <v>9.51</v>
@@ -2800,8 +3116,7 @@
       <c r="K11" s="1"/>
       <c r="M11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="23"/>
+      <c r="Q11" s="20"/>
       <c r="R11" s="1"/>
       <c r="T11" s="12">
         <v>9.51</v>
@@ -2828,8 +3143,7 @@
       <c r="K12" s="1"/>
       <c r="M12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="23"/>
+      <c r="Q12" s="20"/>
       <c r="R12" s="1"/>
       <c r="T12" s="12">
         <v>9.51</v>
@@ -2856,8 +3170,7 @@
       <c r="K13" s="1"/>
       <c r="M13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="23"/>
+      <c r="Q13" s="20"/>
       <c r="R13" s="1"/>
       <c r="T13" s="12">
         <v>9.51</v>
@@ -2884,8 +3197,7 @@
       <c r="K14" s="1"/>
       <c r="M14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="23"/>
+      <c r="Q14" s="20"/>
       <c r="R14" s="1"/>
       <c r="T14" s="12">
         <v>9.51</v>
@@ -2912,8 +3224,7 @@
       <c r="K15" s="1"/>
       <c r="M15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="23"/>
+      <c r="Q15" s="20"/>
       <c r="R15" s="1"/>
       <c r="T15" s="12">
         <v>9.51</v>
@@ -2940,8 +3251,7 @@
       <c r="K16" s="1"/>
       <c r="M16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="23"/>
+      <c r="Q16" s="20"/>
       <c r="R16" s="1"/>
       <c r="T16" s="12">
         <v>9.51</v>
@@ -2968,8 +3278,7 @@
       <c r="K17" s="1"/>
       <c r="M17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="23"/>
+      <c r="Q17" s="20"/>
       <c r="R17" s="1"/>
       <c r="T17" s="12">
         <v>9.51</v>
@@ -2996,8 +3305,7 @@
       <c r="K18" s="1"/>
       <c r="M18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="23"/>
+      <c r="Q18" s="20"/>
       <c r="R18" s="1"/>
       <c r="T18" s="12">
         <v>9.51</v>
@@ -3024,8 +3332,7 @@
       <c r="K19" s="1"/>
       <c r="M19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="23"/>
+      <c r="Q19" s="20"/>
       <c r="R19" s="1"/>
       <c r="T19" s="12">
         <v>9.51</v>
@@ -3052,8 +3359,7 @@
       <c r="K20" s="1"/>
       <c r="M20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="23"/>
+      <c r="Q20" s="20"/>
       <c r="R20" s="1"/>
       <c r="T20" s="12">
         <v>9.51</v>
@@ -3080,8 +3386,7 @@
       <c r="K21" s="1"/>
       <c r="M21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="23"/>
+      <c r="Q21" s="20"/>
       <c r="R21" s="1"/>
       <c r="T21" s="12">
         <v>9.51</v>
@@ -3108,8 +3413,7 @@
       <c r="K22" s="1"/>
       <c r="M22" s="1"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="23"/>
+      <c r="Q22" s="20"/>
       <c r="R22" s="1"/>
       <c r="T22" s="12">
         <v>9.51</v>
@@ -3136,8 +3440,7 @@
       <c r="K23" s="1"/>
       <c r="M23" s="1"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="23"/>
+      <c r="Q23" s="20"/>
       <c r="R23" s="1"/>
       <c r="T23" s="12">
         <v>9.51</v>
@@ -3164,8 +3467,7 @@
       <c r="K24" s="1"/>
       <c r="M24" s="1"/>
       <c r="O24" s="1"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="23"/>
+      <c r="Q24" s="20"/>
       <c r="R24" s="1"/>
       <c r="T24" s="12">
         <v>9.51</v>
@@ -3192,8 +3494,7 @@
       <c r="K25" s="1"/>
       <c r="M25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="23"/>
+      <c r="Q25" s="20"/>
       <c r="R25" s="1"/>
       <c r="T25" s="12">
         <v>9.51</v>
@@ -3220,8 +3521,7 @@
       <c r="K26" s="1"/>
       <c r="M26" s="1"/>
       <c r="O26" s="1"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="23"/>
+      <c r="Q26" s="20"/>
       <c r="R26" s="1"/>
       <c r="T26" s="12">
         <v>9.51</v>
@@ -3248,8 +3548,7 @@
       <c r="K27" s="1"/>
       <c r="M27" s="1"/>
       <c r="O27" s="1"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="23"/>
+      <c r="Q27" s="20"/>
       <c r="R27" s="1"/>
       <c r="T27" s="12">
         <v>9.51</v>
@@ -3276,8 +3575,7 @@
       <c r="K28" s="1"/>
       <c r="M28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="23"/>
+      <c r="Q28" s="20"/>
       <c r="R28" s="1"/>
       <c r="T28" s="12">
         <v>9.51</v>
@@ -3304,8 +3602,7 @@
       <c r="K29" s="1"/>
       <c r="M29" s="1"/>
       <c r="O29" s="1"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="23"/>
+      <c r="Q29" s="20"/>
       <c r="R29" s="1"/>
       <c r="T29" s="12">
         <v>9.51</v>
@@ -3340,7 +3637,7 @@
       <c r="N30" s="4"/>
       <c r="O30" s="2"/>
       <c r="P30" s="4"/>
-      <c r="Q30" s="26"/>
+      <c r="Q30" s="22"/>
       <c r="R30" s="2"/>
       <c r="S30" s="4"/>
       <c r="T30" s="14">
@@ -3368,6 +3665,7 @@
     <hyperlink ref="Z7" r:id="rId5" display="https://www.elvia.no/nettleie/alt-om-nettleiepriser/nettleiepriser-for-bedrifter-og-naering/" xr:uid="{74A79962-4EB6-4A7C-832B-B2E80B4D78E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -3375,9 +3673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABFB50A0-E021-40BB-8D8B-02D73AD8ED8C}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J6" sqref="J6"/>
+      <selection pane="topRight" activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3398,7 +3696,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>34</v>
@@ -3494,7 +3792,7 @@
       <c r="E3" s="1">
         <v>48</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="1">
         <v>71</v>
       </c>
       <c r="G3" s="12">
@@ -3509,10 +3807,10 @@
       <c r="J3" s="12">
         <v>800</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="16">
         <v>45601</v>
       </c>
       <c r="M3" s="3" t="s">
@@ -3535,7 +3833,7 @@
       <c r="E4" s="1">
         <v>36</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="1">
         <v>108</v>
       </c>
       <c r="G4" s="12">
@@ -3550,10 +3848,10 @@
       <c r="J4" s="12">
         <v>800</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="16">
         <v>45601</v>
       </c>
       <c r="M4" s="3" t="s">
@@ -3576,7 +3874,7 @@
       <c r="E5" s="1">
         <v>58</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="1">
         <v>70</v>
       </c>
       <c r="G5" s="12">
@@ -3591,8 +3889,8 @@
       <c r="J5" s="12">
         <v>800</v>
       </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="18">
+      <c r="K5" s="1"/>
+      <c r="L5" s="16">
         <v>45601</v>
       </c>
       <c r="M5" s="3" t="s">
@@ -3615,7 +3913,7 @@
       <c r="E6" s="1">
         <v>51.26</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="1">
         <v>69.91</v>
       </c>
       <c r="G6" s="12">
@@ -3630,10 +3928,10 @@
       <c r="J6" s="12">
         <v>800</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="16">
         <v>45601</v>
       </c>
       <c r="M6" s="3" t="s">
@@ -3656,7 +3954,7 @@
       <c r="E7" s="1">
         <v>44</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="1">
         <v>104</v>
       </c>
       <c r="G7" s="12">
@@ -3671,13 +3969,13 @@
       <c r="J7" s="12">
         <v>800</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="K7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="16">
         <v>45601</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="17" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3697,7 +3995,7 @@
       <c r="J8" s="12">
         <v>800</v>
       </c>
-      <c r="K8" s="16"/>
+      <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
@@ -3717,7 +4015,7 @@
       <c r="J9" s="12">
         <v>800</v>
       </c>
-      <c r="K9" s="16"/>
+      <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
@@ -3737,7 +4035,7 @@
       <c r="J10" s="12">
         <v>800</v>
       </c>
-      <c r="K10" s="16"/>
+      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
@@ -3757,7 +4055,7 @@
       <c r="J11" s="12">
         <v>800</v>
       </c>
-      <c r="K11" s="16"/>
+      <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
@@ -3777,7 +4075,7 @@
       <c r="J12" s="12">
         <v>800</v>
       </c>
-      <c r="K12" s="16"/>
+      <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
@@ -3797,7 +4095,7 @@
       <c r="J13" s="12">
         <v>800</v>
       </c>
-      <c r="K13" s="16"/>
+      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
@@ -3817,7 +4115,7 @@
       <c r="J14" s="12">
         <v>800</v>
       </c>
-      <c r="K14" s="16"/>
+      <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
@@ -3837,7 +4135,7 @@
       <c r="J15" s="12">
         <v>800</v>
       </c>
-      <c r="K15" s="16"/>
+      <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
@@ -3857,7 +4155,7 @@
       <c r="J16" s="12">
         <v>800</v>
       </c>
-      <c r="K16" s="16"/>
+      <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
@@ -3877,7 +4175,7 @@
       <c r="J17" s="12">
         <v>800</v>
       </c>
-      <c r="K17" s="16"/>
+      <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
@@ -3897,7 +4195,7 @@
       <c r="J18" s="12">
         <v>800</v>
       </c>
-      <c r="K18" s="16"/>
+      <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
@@ -3917,7 +4215,7 @@
       <c r="J19" s="12">
         <v>800</v>
       </c>
-      <c r="K19" s="16"/>
+      <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
@@ -3937,7 +4235,7 @@
       <c r="J20" s="12">
         <v>800</v>
       </c>
-      <c r="K20" s="16"/>
+      <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
@@ -3957,7 +4255,7 @@
       <c r="J21" s="12">
         <v>800</v>
       </c>
-      <c r="K21" s="16"/>
+      <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
@@ -3977,7 +4275,7 @@
       <c r="J22" s="12">
         <v>800</v>
       </c>
-      <c r="K22" s="16"/>
+      <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
@@ -3997,7 +4295,7 @@
       <c r="J23" s="12">
         <v>800</v>
       </c>
-      <c r="K23" s="16"/>
+      <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
@@ -4017,7 +4315,7 @@
       <c r="J24" s="12">
         <v>800</v>
       </c>
-      <c r="K24" s="16"/>
+      <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
@@ -4037,7 +4335,7 @@
       <c r="J25" s="12">
         <v>800</v>
       </c>
-      <c r="K25" s="16"/>
+      <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
@@ -4057,7 +4355,7 @@
       <c r="J26" s="12">
         <v>800</v>
       </c>
-      <c r="K26" s="16"/>
+      <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
@@ -4077,7 +4375,7 @@
       <c r="J27" s="12">
         <v>800</v>
       </c>
-      <c r="K27" s="16"/>
+      <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
@@ -4097,7 +4395,7 @@
       <c r="J28" s="12">
         <v>800</v>
       </c>
-      <c r="K28" s="16"/>
+      <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
@@ -4117,7 +4415,7 @@
       <c r="J29" s="12">
         <v>800</v>
       </c>
-      <c r="K29" s="16"/>
+      <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
@@ -4140,7 +4438,7 @@
       <c r="J30" s="14">
         <v>800</v>
       </c>
-      <c r="K30" s="17"/>
+      <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>

</xml_diff>